<commit_message>
Updated Tableau file for updated data connection
</commit_message>
<xml_diff>
--- a/2013 Election Results.xlsx
+++ b/2013 Election Results.xlsx
@@ -42,9 +42,6 @@
     <t>Mayor</t>
   </si>
   <si>
-    <t>Charyl L. Drab</t>
-  </si>
-  <si>
     <t>918 of 918</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>887 of 887</t>
   </si>
   <si>
-    <t>Mike "Griff" Griffin</t>
-  </si>
-  <si>
     <t>City Council At-Large Pos. 2</t>
   </si>
   <si>
@@ -280,6 +274,12 @@
   </si>
   <si>
     <t>Winner (Runoff)</t>
+  </si>
+  <si>
+    <t>Michael Griffin</t>
+  </si>
+  <si>
+    <t>Charyl Drab</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -538,9 +538,6 @@
     <xf numFmtId="10" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -568,9 +565,6 @@
     <xf numFmtId="3" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -583,9 +577,6 @@
     <xf numFmtId="9" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -593,6 +584,28 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1122,14 +1135,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" style="13" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" style="13" customWidth="1"/>
     <col min="5" max="5" width="21" style="13" customWidth="1"/>
@@ -1162,15 +1175,15 @@
         <v>6</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="23">
         <v>71462</v>
@@ -1180,65 +1193,65 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="13">
         <v>2013</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="56">
+      <c r="A3" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="55">
         <v>66627</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="61">
+      <c r="D3" s="50"/>
+      <c r="E3" s="59">
         <v>0.48199999999999998</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>9</v>
+      <c r="F3" s="50" t="s">
+        <v>8</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="13">
         <v>2013</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:8" s="68" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="65">
+        <v>50426</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="66">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="F4" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="41">
-        <v>50426</v>
-      </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="37">
+      <c r="G4" s="67"/>
+      <c r="H4" s="68">
         <v>2013</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" s="4">
         <v>78294</v>
@@ -1248,10 +1261,10 @@
         <v>0.60799999999999998</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="13">
         <v>2013</v>
@@ -1259,10 +1272,10 @@
     </row>
     <row r="6" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="4">
         <v>46765</v>
@@ -1272,7 +1285,7 @@
         <v>0.376</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="13">
@@ -1281,10 +1294,10 @@
     </row>
     <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4">
         <v>50452</v>
@@ -1294,10 +1307,10 @@
         <v>0.40400000000000003</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="13">
         <v>2013</v>
@@ -1305,10 +1318,10 @@
     </row>
     <row r="8" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="6">
         <v>19936</v>
@@ -1318,7 +1331,7 @@
         <v>0.158</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="13">
@@ -1327,10 +1340,10 @@
     </row>
     <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="41">
         <v>7745</v>
@@ -1340,7 +1353,7 @@
         <v>6.2E-2</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="43"/>
       <c r="H9" s="37">
@@ -1349,12 +1362,12 @@
     </row>
     <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="54">
+        <v>51</v>
+      </c>
+      <c r="C10" s="53">
         <v>11257</v>
       </c>
       <c r="D10" s="46"/>
@@ -1362,7 +1375,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="F10" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="43"/>
       <c r="H10" s="37">
@@ -1371,10 +1384,10 @@
     </row>
     <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C11" s="4">
         <v>22123</v>
@@ -1384,7 +1397,7 @@
         <v>0.16900000000000001</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="13">
@@ -1393,10 +1406,10 @@
     </row>
     <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="C12" s="6">
         <v>37201</v>
@@ -1406,10 +1419,10 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="13">
         <v>2013</v>
@@ -1417,10 +1430,10 @@
     </row>
     <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="23">
         <v>23174</v>
@@ -1430,7 +1443,7 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="13">
@@ -1439,10 +1452,10 @@
     </row>
     <row r="14" spans="1:8" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="4">
         <v>20992</v>
@@ -1452,7 +1465,7 @@
         <v>0.161</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="13">
@@ -1461,10 +1474,10 @@
     </row>
     <row r="15" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="23">
         <v>16054</v>
@@ -1474,7 +1487,7 @@
         <v>0.122</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="13">
@@ -1483,10 +1496,10 @@
     </row>
     <row r="16" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C16" s="23">
         <v>108764</v>
@@ -1496,10 +1509,10 @@
         <v>0.81399999999999995</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="13">
         <v>2013</v>
@@ -1507,10 +1520,10 @@
     </row>
     <row r="17" spans="1:8" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="4">
         <v>24824</v>
@@ -1520,7 +1533,7 @@
         <v>0.186</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="13">
@@ -1529,10 +1542,10 @@
     </row>
     <row r="18" spans="1:8" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" s="4">
         <v>41342</v>
@@ -1542,7 +1555,7 @@
         <v>0.32400000000000001</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="13">
@@ -1551,10 +1564,10 @@
     </row>
     <row r="19" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="6">
         <v>70029</v>
@@ -1564,10 +1577,10 @@
         <v>0.54800000000000004</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" s="13">
         <v>2013</v>
@@ -1575,10 +1588,10 @@
     </row>
     <row r="20" spans="1:8" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20" s="41">
         <v>16511</v>
@@ -1588,7 +1601,7 @@
         <v>0.128</v>
       </c>
       <c r="F20" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="43"/>
       <c r="H20" s="37">
@@ -1597,10 +1610,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>16</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="C21" s="17">
         <v>956</v>
@@ -1610,7 +1623,7 @@
         <v>7.8799999999999995E-2</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="13">
@@ -1619,10 +1632,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="21">
         <v>3538</v>
@@ -1632,10 +1645,10 @@
         <v>0.29170000000000001</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H22" s="13">
         <v>2013</v>
@@ -1643,10 +1656,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="21">
         <v>4613</v>
@@ -1656,7 +1669,7 @@
         <v>0.38040000000000002</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="13">
@@ -1665,10 +1678,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="45">
         <v>2391</v>
@@ -1678,7 +1691,7 @@
         <v>0.17710000000000001</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G24" s="36"/>
       <c r="H24" s="37">
@@ -1687,10 +1700,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C25" s="29">
         <v>630</v>
@@ -1700,7 +1713,7 @@
         <v>5.1900000000000002E-2</v>
       </c>
       <c r="F25" s="29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="13">
@@ -1708,46 +1721,46 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49" t="s">
+      <c r="A26" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="48">
+        <v>961</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="57">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F26" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="G26" s="61"/>
+      <c r="H26" s="13">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="49">
-        <v>961</v>
-      </c>
-      <c r="D26" s="49"/>
-      <c r="E26" s="59">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="F26" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="64"/>
-      <c r="H26" s="13">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="50" t="s">
+      <c r="C27" s="54">
+        <v>7245</v>
+      </c>
+      <c r="D27" s="49"/>
+      <c r="E27" s="58">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="F27" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="55">
-        <v>7245</v>
-      </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="60">
-        <v>0.59199999999999997</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="65" t="s">
-        <v>12</v>
+      <c r="G27" s="62" t="s">
+        <v>11</v>
       </c>
       <c r="H27" s="13">
         <v>2013</v>
@@ -1755,10 +1768,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="31">
         <v>2747</v>
@@ -1768,7 +1781,7 @@
         <v>0.224</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="13">
@@ -1777,10 +1790,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="44">
         <v>1278</v>
@@ -1790,7 +1803,7 @@
         <v>0.105</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G29" s="36"/>
       <c r="H29" s="37">
@@ -1799,10 +1812,10 @@
     </row>
     <row r="30" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3">
         <v>730</v>
@@ -1812,7 +1825,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="13">
@@ -1821,10 +1834,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" s="21">
         <v>1882</v>
@@ -1834,7 +1847,7 @@
         <v>0.1095</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="13">
@@ -1843,10 +1856,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C32" s="21">
         <v>1151</v>
@@ -1856,7 +1869,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="13">
@@ -1865,10 +1878,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="34">
         <v>467</v>
@@ -1878,7 +1891,7 @@
         <v>2.7199999999999998E-2</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G33" s="36"/>
       <c r="H33" s="37">
@@ -1887,10 +1900,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="18">
         <v>7372</v>
@@ -1900,10 +1913,10 @@
         <v>0.42899999999999999</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H34" s="13">
         <v>2013</v>
@@ -1911,10 +1924,10 @@
     </row>
     <row r="35" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" s="4">
         <v>2469</v>
@@ -1924,10 +1937,10 @@
         <v>0.14369999999999999</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H35" s="13">
         <v>2013</v>
@@ -1935,10 +1948,10 @@
     </row>
     <row r="36" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C36" s="46">
         <v>165</v>
@@ -1948,7 +1961,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
       <c r="F36" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G36" s="43"/>
       <c r="H36" s="37">
@@ -1957,10 +1970,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="17">
         <v>464</v>
@@ -1970,7 +1983,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="13">
@@ -1979,10 +1992,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="1">
         <v>263</v>
@@ -1992,7 +2005,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="13">
@@ -2001,10 +2014,10 @@
     </row>
     <row r="39" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="24">
         <v>731</v>
@@ -2014,7 +2027,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G39" s="28"/>
       <c r="H39" s="13">
@@ -2023,10 +2036,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="46">
         <v>424</v>
@@ -2036,7 +2049,7 @@
         <v>2.47E-2</v>
       </c>
       <c r="F40" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G40" s="43"/>
       <c r="H40" s="37">
@@ -2045,10 +2058,10 @@
     </row>
     <row r="41" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>27</v>
       </c>
       <c r="C41" s="21">
         <v>1068</v>
@@ -2058,7 +2071,7 @@
         <v>6.2100000000000002E-2</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="13">
@@ -2067,10 +2080,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C42" s="6">
         <v>2986</v>
@@ -2089,10 +2102,10 @@
     </row>
     <row r="43" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C43" s="4">
         <v>3193</v>
@@ -2105,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H43" s="13">
         <v>2013</v>
@@ -2113,10 +2126,10 @@
     </row>
     <row r="44" spans="1:8" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C44" s="4">
         <v>3641</v>
@@ -2126,7 +2139,7 @@
         <v>0.1721</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G44" s="10"/>
       <c r="H44" s="13">
@@ -2135,10 +2148,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C45" s="6">
         <v>17518</v>
@@ -2148,10 +2161,10 @@
         <v>0.82789999999999997</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H45" s="13">
         <v>2013</v>
@@ -2159,10 +2172,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="6">
         <v>2118</v>
@@ -2172,7 +2185,7 @@
         <v>0.24840000000000001</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G46" s="9"/>
       <c r="H46" s="13">
@@ -2181,10 +2194,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C47" s="4">
         <v>2313</v>
@@ -2194,7 +2207,7 @@
         <v>0.26929999999999998</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G47" s="10"/>
       <c r="H47" s="13">
@@ -2203,10 +2216,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C48" s="4">
         <v>1973</v>
@@ -2216,7 +2229,7 @@
         <v>0.23139999999999999</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G48" s="10"/>
       <c r="H48" s="13">
@@ -2225,10 +2238,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" s="6">
         <v>2138</v>
@@ -2238,10 +2251,10 @@
         <v>0.25090000000000001</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H49" s="13">
         <v>2013</v>
@@ -2252,7 +2265,7 @@
         <v>7</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C50" s="18">
         <v>97968</v>
@@ -2262,56 +2275,56 @@
         <v>0.56799999999999995</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H50" s="13">
         <v>2013</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="53">
+      <c r="B51" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="52">
         <v>48551</v>
       </c>
-      <c r="D51" s="49"/>
-      <c r="E51" s="59">
+      <c r="D51" s="48"/>
+      <c r="E51" s="57">
         <v>0.28199999999999997</v>
       </c>
-      <c r="F51" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="64"/>
+      <c r="F51" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="61"/>
       <c r="H51" s="13">
         <v>2013</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="48" t="s">
+    <row r="52" spans="1:8" s="68" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="48" t="s">
+      <c r="B52" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="69">
+        <v>784</v>
+      </c>
+      <c r="D52" s="69"/>
+      <c r="E52" s="70">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F52" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="48">
-        <v>784</v>
-      </c>
-      <c r="D52" s="48"/>
-      <c r="E52" s="58">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F52" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="63"/>
-      <c r="H52" s="37">
+      <c r="G52" s="71"/>
+      <c r="H52" s="68">
         <v>2013</v>
       </c>
     </row>
@@ -2320,7 +2333,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C53" s="38">
         <v>833</v>
@@ -2330,7 +2343,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F53" s="38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G53" s="36"/>
       <c r="H53" s="37">
@@ -2342,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C54" s="31">
         <v>1738</v>
@@ -2352,7 +2365,7 @@
         <v>0.01</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G54" s="16"/>
       <c r="H54" s="13">
@@ -2364,7 +2377,7 @@
         <v>7</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C55" s="30">
         <v>18350</v>
@@ -2374,7 +2387,7 @@
         <v>0.106</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G55" s="20"/>
       <c r="H55" s="13">
@@ -2386,7 +2399,7 @@
         <v>7</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C56" s="45">
         <v>1223</v>
@@ -2396,7 +2409,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="F56" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G56" s="36"/>
       <c r="H56" s="37">
@@ -2408,7 +2421,7 @@
         <v>7</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C57" s="45">
         <v>1191</v>
@@ -2418,7 +2431,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="F57" s="34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G57" s="36"/>
       <c r="H57" s="37">
@@ -2426,23 +2439,23 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="52" t="s">
+      <c r="A58" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="57">
+      <c r="B58" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="56">
         <v>1810</v>
       </c>
-      <c r="D58" s="52"/>
-      <c r="E58" s="62">
+      <c r="D58" s="51"/>
+      <c r="E58" s="60">
         <v>0.01</v>
       </c>
-      <c r="F58" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G58" s="66"/>
+      <c r="F58" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="63"/>
       <c r="H58" s="13">
         <v>2013</v>
       </c>

</xml_diff>